<commit_message>
minor up - fix su stati esteri/codicifiscali
</commit_message>
<xml_diff>
--- a/Attestati Corsi di Formazione/report_gen_data/db/new_master.xlsx
+++ b/Attestati Corsi di Formazione/report_gen_data/db/new_master.xlsx
@@ -328,7 +328,7 @@
   <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
@@ -565,6 +565,9 @@
           <t>elettrohertz</t>
         </is>
       </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -602,6 +605,9 @@
           <t>elettrohertz</t>
         </is>
       </c>
+      <c r="H6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -639,6 +645,14 @@
           <t>elettrohertz</t>
         </is>
       </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>petrignani</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -676,6 +690,9 @@
           <t>elettrohertz</t>
         </is>
       </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -713,6 +730,9 @@
           <t>elettrohertz</t>
         </is>
       </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -750,6 +770,9 @@
           <t>elettrohertz</t>
         </is>
       </c>
+      <c r="H10" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -787,6 +810,9 @@
           <t>elettrohertz</t>
         </is>
       </c>
+      <c r="H11" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -819,6 +845,9 @@
           <t>elettrohertz</t>
         </is>
       </c>
+      <c r="H12" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -856,6 +885,9 @@
           <t>chef-and-go</t>
         </is>
       </c>
+      <c r="H13" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -893,6 +925,14 @@
           <t>chef-and-go</t>
         </is>
       </c>
+      <c r="H14" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>petrignani</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -994,6 +1034,7 @@
           <t>chef-and-go</t>
         </is>
       </c>
+      <c r="I17" s="4" t="n"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">

</xml_diff>